<commit_message>
Changed the test data in the driver sheet
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/SophieAutomation.xlsx
+++ b/TestDataAndResults/TestData/SophieAutomation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3BCE6A-6F26-4D65-ACCD-2DB08400D9FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8477B9-B660-4478-965D-1C32BB43AD9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1098,6 +1098,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1137,7 +1138,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1507,7 +1507,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1521,22 +1521,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" ht="14.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="14.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" ht="14.25">
       <c r="A3" s="10"/>
@@ -1573,7 +1573,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -1588,7 +1588,7 @@
         <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1603,7 +1603,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1618,7 +1618,7 @@
         <v>282</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -1667,38 +1667,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
@@ -2413,7 +2413,7 @@
       <c r="D37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F37" s="3"/>
@@ -2455,7 +2455,7 @@
       <c r="D39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F39" s="3"/>
@@ -2595,38 +2595,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -3571,7 +3571,7 @@
       <c r="D48" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F48" s="3"/>
@@ -3613,7 +3613,7 @@
       <c r="D50" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F50" s="3"/>
@@ -3756,38 +3756,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -4606,7 +4606,7 @@
       <c r="D42" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F42" s="21"/>
@@ -4648,7 +4648,7 @@
       <c r="D44" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="23" t="s">
         <v>266</v>
       </c>
       <c r="F44" s="21"/>
@@ -4790,36 +4790,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -6105,36 +6105,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
@@ -7029,36 +7029,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="31"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">

</xml_diff>